<commit_message>
Add information about num of executiontime > 120s
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure6.xlsx
+++ b/paper/pldi21/img/figure6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yundongjun/PLRG/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5ED05C-1658-7346-8386-0CBA1AE12A38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA443CB-F0BD-5949-9416-7E05DAE0D848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="4" xr2:uid="{6D571640-1E5C-7D4E-B475-B88EE9F06437}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="22">
   <si>
     <t>DS</t>
   </si>
@@ -101,6 +101,10 @@
   </si>
   <si>
     <t>no-DS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>More than 2m</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4086,16 +4090,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>354736</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>58133</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>888136</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>134333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>814857</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>51387</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>395757</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4122,16 +4126,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>78282</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>86167</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>611682</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>162367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>663248</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>188583</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>244148</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>36183</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -4167,7 +4171,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10555782" y="1914967"/>
+              <a:off x="12994182" y="2219767"/>
               <a:ext cx="584966" cy="3074216"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4200,16 +4204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>718785</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>27171</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>299685</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>103371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>53662</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>165457</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>587062</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>13057</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20723,15 +20727,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB22A503-B58D-B041-B089-126B049701B1}">
-  <dimension ref="A1:F301"/>
+  <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -20750,8 +20757,11 @@
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20771,8 +20781,15 @@
         <f>LOG(D2,2)</f>
         <v>4.2055024764274478</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <f>B301-B121</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -20792,8 +20809,15 @@
         <f t="shared" ref="E3:E66" si="0">LOG(D3,2)</f>
         <v>4.080345546108064</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <f>C301-C121</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -20814,7 +20838,7 @@
         <v>4.1567556261915053</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -20835,7 +20859,7 @@
         <v>4.1369829770941378</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -20856,7 +20880,7 @@
         <v>4.0067010801584519</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -20877,7 +20901,7 @@
         <v>4.1454270414869967</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -20898,7 +20922,7 @@
         <v>3.9679123790283608</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20919,7 +20943,7 @@
         <v>4.18361105784766</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20940,7 +20964,7 @@
         <v>4.1657079503378407</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20961,7 +20985,7 @@
         <v>4.1465745141649313</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -20982,7 +21006,7 @@
         <v>4.1752657987624398</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -21003,7 +21027,7 @@
         <v>4.2465846684179445</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -21024,7 +21048,7 @@
         <v>4.0728476871987311</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -21045,7 +21069,7 @@
         <v>5.3746751383336999</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Generate figure6 png file
</commit_message>
<xml_diff>
--- a/paper/pldi21/img/figure6.xlsx
+++ b/paper/pldi21/img/figure6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yundongjun/PLRG/safe/paper/pldi21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA443CB-F0BD-5949-9416-7E05DAE0D848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFC0102-FF8D-3940-91F4-5D1D6998C0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="4" xr2:uid="{6D571640-1E5C-7D4E-B475-B88EE9F06437}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="26">
   <si>
     <t>DS</t>
   </si>
@@ -105,6 +105,22 @@
   </si>
   <si>
     <t>More than 2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1788,7 +1804,23 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>time (s)</a:t>
+                  <a:t>time (s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>ec.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2352,7 +2384,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4127,15 +4159,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>611682</xdr:colOff>
+      <xdr:colOff>889628</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>162367</xdr:rowOff>
+      <xdr:rowOff>25532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>244148</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>36183</xdr:rowOff>
+      <xdr:colOff>522094</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>125981</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -4171,8 +4203,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12994182" y="2219767"/>
-              <a:ext cx="584966" cy="3074216"/>
+              <a:off x="13551143" y="2065229"/>
+              <a:ext cx="586035" cy="3046678"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4541,8 +4573,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D270"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5429,7 +5461,7 @@
         <v>19.081668885929869</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>69</v>
       </c>
@@ -6591,7 +6623,7 @@
         <v>17.655061841502519</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1">
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>161</v>
       </c>
@@ -8329,98 +8361,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D270" xr:uid="{6D5303D2-6B0B-8941-9672-9FEE8B1AC290}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="10.15"/>
-        <filter val="13.74"/>
-        <filter val="2.11"/>
-        <filter val="2.12"/>
-        <filter val="2.13"/>
-        <filter val="2.14"/>
-        <filter val="2.15"/>
-        <filter val="2.16"/>
-        <filter val="2.17"/>
-        <filter val="2.18"/>
-        <filter val="2.19"/>
-        <filter val="2.20"/>
-        <filter val="2.21"/>
-        <filter val="2.22"/>
-        <filter val="2.23"/>
-        <filter val="2.24"/>
-        <filter val="2.25"/>
-        <filter val="2.26"/>
-        <filter val="2.27"/>
-        <filter val="2.28"/>
-        <filter val="2.29"/>
-        <filter val="2.30"/>
-        <filter val="2.31"/>
-        <filter val="2.32"/>
-        <filter val="2.33"/>
-        <filter val="2.34"/>
-        <filter val="2.35"/>
-        <filter val="2.36"/>
-        <filter val="2.38"/>
-        <filter val="2.39"/>
-        <filter val="2.40"/>
-        <filter val="2.41"/>
-        <filter val="2.43"/>
-        <filter val="2.44"/>
-        <filter val="2.45"/>
-        <filter val="2.46"/>
-        <filter val="2.48"/>
-        <filter val="2.49"/>
-        <filter val="2.50"/>
-        <filter val="2.51"/>
-        <filter val="2.55"/>
-        <filter val="2.56"/>
-        <filter val="2.57"/>
-        <filter val="2.60"/>
-        <filter val="2.61"/>
-        <filter val="2.63"/>
-        <filter val="2.64"/>
-        <filter val="2.65"/>
-        <filter val="2.68"/>
-        <filter val="2.70"/>
-        <filter val="2.71"/>
-        <filter val="2.72"/>
-        <filter val="2.73"/>
-        <filter val="2.79"/>
-        <filter val="2.81"/>
-        <filter val="2.83"/>
-        <filter val="2.84"/>
-        <filter val="2.88"/>
-        <filter val="2.92"/>
-        <filter val="2.95"/>
-        <filter val="2.99"/>
-        <filter val="3.01"/>
-        <filter val="3.03"/>
-        <filter val="3.04"/>
-        <filter val="3.16"/>
-        <filter val="3.18"/>
-        <filter val="3.20"/>
-        <filter val="3.29"/>
-        <filter val="3.35"/>
-        <filter val="3.38"/>
-        <filter val="3.47"/>
-        <filter val="3.64"/>
-        <filter val="3.91"/>
-        <filter val="4.11"/>
-        <filter val="4.25"/>
-        <filter val="4.71"/>
-        <filter val="4.87"/>
-        <filter val="4.92"/>
-        <filter val="4.94"/>
-        <filter val="43.59"/>
-        <filter val="5.22"/>
-        <filter val="5.24"/>
-        <filter val="5.34"/>
-        <filter val="5.49"/>
-        <filter val="6.12"/>
-        <filter val="6.17"/>
-        <filter val="6.29"/>
-        <filter val="7.90"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="119.15"/>
@@ -8555,6 +8495,7 @@
         <filter val="45.10"/>
         <filter val="45.98"/>
         <filter val="47.17"/>
+        <filter val="47.68"/>
         <filter val="47.83"/>
         <filter val="47.93"/>
         <filter val="48.10"/>
@@ -8576,6 +8517,7 @@
         <filter val="69.74"/>
         <filter val="73.15"/>
         <filter val="76.44"/>
+        <filter val="76.98"/>
         <filter val="78.75"/>
         <filter val="81.38"/>
         <filter val="83.79"/>
@@ -8597,7 +8539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68A2F5D-D56E-6847-8151-EE180B0E3B43}">
   <dimension ref="A1:J556"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
+    <sheetView topLeftCell="A110" zoomScale="94" workbookViewId="0">
       <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
@@ -17490,10 +17432,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A9B793-ECBF-1646-8B89-61EB194F07F8}">
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -17501,7 +17443,7 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -17517,8 +17459,20 @@
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17534,8 +17488,24 @@
       <c r="E2" s="1">
         <v>18.449406175771969</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1">
+        <f>MIN($E2:$E199)</f>
+        <v>0.90111503693846662</v>
+      </c>
+      <c r="G2" s="1">
+        <f>MAX($E2:$E199)</f>
+        <v>54.975995075913005</v>
+      </c>
+      <c r="H2" s="1">
+        <f>MEDIAN($E2:$E199)</f>
+        <v>17.843194408899997</v>
+      </c>
+      <c r="I2" s="1">
+        <f>AVERAGE($E2:$E199)</f>
+        <v>19.964721239676258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -17552,7 +17522,7 @@
         <v>16.916339869281046</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -17569,7 +17539,7 @@
         <v>17.83643798273512</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -17586,7 +17556,7 @@
         <v>17.593650793650792</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -17603,7 +17573,7 @@
         <v>16.074490220557639</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -17620,7 +17590,7 @@
         <v>17.696928014672167</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -17637,7 +17607,7 @@
         <v>15.648065173116088</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -17654,7 +17624,7 @@
         <v>18.171568627450981</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -17671,7 +17641,7 @@
         <v>17.947462154942119</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -17688,7 +17658,7 @@
         <v>17.711009174311926</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -17705,7 +17675,7 @@
         <v>18.066758747697971</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -17722,7 +17692,7 @@
         <v>18.982323232323232</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -17739,7 +17709,7 @@
         <v>16.828651685393258</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -17756,7 +17726,7 @@
         <v>41.489522212908632</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -19949,7 +19919,10 @@
         <v>16.927586206896553</v>
       </c>
     </row>
-    <row r="145" spans="2:5">
+    <row r="145" spans="1:5">
+      <c r="A145">
+        <v>144</v>
+      </c>
       <c r="B145">
         <v>225</v>
       </c>
@@ -19963,7 +19936,10 @@
         <v>17.574774034511091</v>
       </c>
     </row>
-    <row r="146" spans="2:5">
+    <row r="146" spans="1:5">
+      <c r="A146">
+        <v>145</v>
+      </c>
       <c r="B146">
         <v>226</v>
       </c>
@@ -19977,7 +19953,10 @@
         <v>18.051594746716695</v>
       </c>
     </row>
-    <row r="147" spans="2:5">
+    <row r="147" spans="1:5">
+      <c r="A147">
+        <v>146</v>
+      </c>
       <c r="B147">
         <v>227</v>
       </c>
@@ -19991,7 +19970,10 @@
         <v>17.838782924613987</v>
       </c>
     </row>
-    <row r="148" spans="2:5">
+    <row r="148" spans="1:5">
+      <c r="A148">
+        <v>147</v>
+      </c>
       <c r="B148">
         <v>231</v>
       </c>
@@ -20005,7 +19987,10 @@
         <v>17.457923008057296</v>
       </c>
     </row>
-    <row r="149" spans="2:5">
+    <row r="149" spans="1:5">
+      <c r="A149">
+        <v>148</v>
+      </c>
       <c r="B149">
         <v>233</v>
       </c>
@@ -20019,7 +20004,10 @@
         <v>33.822527015793845</v>
       </c>
     </row>
-    <row r="150" spans="2:5">
+    <row r="150" spans="1:5">
+      <c r="A150">
+        <v>149</v>
+      </c>
       <c r="B150">
         <v>234</v>
       </c>
@@ -20033,7 +20021,10 @@
         <v>17.774384685505925</v>
       </c>
     </row>
-    <row r="151" spans="2:5">
+    <row r="151" spans="1:5">
+      <c r="A151">
+        <v>150</v>
+      </c>
       <c r="B151">
         <v>235</v>
       </c>
@@ -20047,7 +20038,10 @@
         <v>38.814634146341461</v>
       </c>
     </row>
-    <row r="152" spans="2:5">
+    <row r="152" spans="1:5">
+      <c r="A152">
+        <v>151</v>
+      </c>
       <c r="B152">
         <v>236</v>
       </c>
@@ -20061,7 +20055,10 @@
         <v>18.03268876611418</v>
       </c>
     </row>
-    <row r="153" spans="2:5">
+    <row r="153" spans="1:5">
+      <c r="A153">
+        <v>152</v>
+      </c>
       <c r="B153">
         <v>237</v>
       </c>
@@ -20075,7 +20072,10 @@
         <v>16.859124403987863</v>
       </c>
     </row>
-    <row r="154" spans="2:5">
+    <row r="154" spans="1:5">
+      <c r="A154">
+        <v>153</v>
+      </c>
       <c r="B154">
         <v>238</v>
       </c>
@@ -20089,7 +20089,10 @@
         <v>21.212871287128714</v>
       </c>
     </row>
-    <row r="155" spans="2:5">
+    <row r="155" spans="1:5">
+      <c r="A155">
+        <v>154</v>
+      </c>
       <c r="B155">
         <v>239</v>
       </c>
@@ -20103,7 +20106,10 @@
         <v>22.729992229992231</v>
       </c>
     </row>
-    <row r="156" spans="2:5">
+    <row r="156" spans="1:5">
+      <c r="A156">
+        <v>155</v>
+      </c>
       <c r="B156">
         <v>240</v>
       </c>
@@ -20117,7 +20123,10 @@
         <v>25.791960507757405</v>
       </c>
     </row>
-    <row r="157" spans="2:5">
+    <row r="157" spans="1:5">
+      <c r="A157">
+        <v>156</v>
+      </c>
       <c r="B157">
         <v>241</v>
       </c>
@@ -20131,7 +20140,10 @@
         <v>31.845950413223143</v>
       </c>
     </row>
-    <row r="158" spans="2:5">
+    <row r="158" spans="1:5">
+      <c r="A158">
+        <v>157</v>
+      </c>
       <c r="B158">
         <v>242</v>
       </c>
@@ -20145,7 +20157,10 @@
         <v>20.1636553161918</v>
       </c>
     </row>
-    <row r="159" spans="2:5">
+    <row r="159" spans="1:5">
+      <c r="A159">
+        <v>158</v>
+      </c>
       <c r="B159">
         <v>243</v>
       </c>
@@ -20159,7 +20174,10 @@
         <v>17.154630039875943</v>
       </c>
     </row>
-    <row r="160" spans="2:5">
+    <row r="160" spans="1:5">
+      <c r="A160">
+        <v>159</v>
+      </c>
       <c r="B160">
         <v>248</v>
       </c>
@@ -20173,7 +20191,10 @@
         <v>21.657712305025996</v>
       </c>
     </row>
-    <row r="161" spans="2:5">
+    <row r="161" spans="1:5">
+      <c r="A161">
+        <v>160</v>
+      </c>
       <c r="B161">
         <v>250</v>
       </c>
@@ -20187,7 +20208,10 @@
         <v>17.814147018030514</v>
       </c>
     </row>
-    <row r="162" spans="2:5">
+    <row r="162" spans="1:5">
+      <c r="A162">
+        <v>161</v>
+      </c>
       <c r="B162">
         <v>251</v>
       </c>
@@ -20201,7 +20225,10 @@
         <v>18.164396430248942</v>
       </c>
     </row>
-    <row r="163" spans="2:5">
+    <row r="163" spans="1:5">
+      <c r="A163">
+        <v>162</v>
+      </c>
       <c r="B163">
         <v>252</v>
       </c>
@@ -20215,7 +20242,10 @@
         <v>17.614837849844516</v>
       </c>
     </row>
-    <row r="164" spans="2:5">
+    <row r="164" spans="1:5">
+      <c r="A164">
+        <v>163</v>
+      </c>
       <c r="B164">
         <v>253</v>
       </c>
@@ -20229,7 +20259,10 @@
         <v>18.344277673545964</v>
       </c>
     </row>
-    <row r="165" spans="2:5">
+    <row r="165" spans="1:5">
+      <c r="A165">
+        <v>164</v>
+      </c>
       <c r="B165">
         <v>254</v>
       </c>
@@ -20243,7 +20276,10 @@
         <v>17.465199820386172</v>
       </c>
     </row>
-    <row r="166" spans="2:5">
+    <row r="166" spans="1:5">
+      <c r="A166">
+        <v>165</v>
+      </c>
       <c r="B166">
         <v>256</v>
       </c>
@@ -20257,7 +20293,10 @@
         <v>17.875406787540683</v>
       </c>
     </row>
-    <row r="167" spans="2:5">
+    <row r="167" spans="1:5">
+      <c r="A167">
+        <v>166</v>
+      </c>
       <c r="B167">
         <v>257</v>
       </c>
@@ -20271,7 +20310,10 @@
         <v>17.594183445190158</v>
       </c>
     </row>
-    <row r="168" spans="2:5">
+    <row r="168" spans="1:5">
+      <c r="A168">
+        <v>167</v>
+      </c>
       <c r="B168">
         <v>258</v>
       </c>
@@ -20285,7 +20327,10 @@
         <v>24.873461538461541</v>
       </c>
     </row>
-    <row r="169" spans="2:5">
+    <row r="169" spans="1:5">
+      <c r="A169">
+        <v>168</v>
+      </c>
       <c r="B169">
         <v>260</v>
       </c>
@@ -20299,7 +20344,10 @@
         <v>18.480018373909051</v>
       </c>
     </row>
-    <row r="170" spans="2:5">
+    <row r="170" spans="1:5">
+      <c r="A170">
+        <v>169</v>
+      </c>
       <c r="B170">
         <v>261</v>
       </c>
@@ -20313,7 +20361,10 @@
         <v>18.607455131155085</v>
       </c>
     </row>
-    <row r="171" spans="2:5">
+    <row r="171" spans="1:5">
+      <c r="A171">
+        <v>170</v>
+      </c>
       <c r="B171">
         <v>262</v>
       </c>
@@ -20327,7 +20378,10 @@
         <v>44.131637168141587</v>
       </c>
     </row>
-    <row r="172" spans="2:5">
+    <row r="172" spans="1:5">
+      <c r="A172">
+        <v>171</v>
+      </c>
       <c r="B172">
         <v>266</v>
       </c>
@@ -20341,7 +20395,10 @@
         <v>17.189081225033288</v>
       </c>
     </row>
-    <row r="173" spans="2:5">
+    <row r="173" spans="1:5">
+      <c r="A173">
+        <v>172</v>
+      </c>
       <c r="B173">
         <v>267</v>
       </c>
@@ -20355,7 +20412,10 @@
         <v>20.985696771557006</v>
       </c>
     </row>
-    <row r="174" spans="2:5">
+    <row r="174" spans="1:5">
+      <c r="A174">
+        <v>173</v>
+      </c>
       <c r="B174">
         <v>268</v>
       </c>
@@ -20369,7 +20429,10 @@
         <v>18.65560538116592</v>
       </c>
     </row>
-    <row r="175" spans="2:5">
+    <row r="175" spans="1:5">
+      <c r="A175">
+        <v>174</v>
+      </c>
       <c r="B175">
         <v>269</v>
       </c>
@@ -20383,7 +20446,10 @@
         <v>17.353270223752151</v>
       </c>
     </row>
-    <row r="176" spans="2:5">
+    <row r="176" spans="1:5">
+      <c r="A176">
+        <v>175</v>
+      </c>
       <c r="B176">
         <v>271</v>
       </c>
@@ -20397,7 +20463,10 @@
         <v>17.875567665758403</v>
       </c>
     </row>
-    <row r="177" spans="2:5">
+    <row r="177" spans="1:5">
+      <c r="A177">
+        <v>176</v>
+      </c>
       <c r="B177">
         <v>273</v>
       </c>
@@ -20411,7 +20480,10 @@
         <v>17.904191616766465</v>
       </c>
     </row>
-    <row r="178" spans="2:5">
+    <row r="178" spans="1:5">
+      <c r="A178">
+        <v>177</v>
+      </c>
       <c r="B178">
         <v>274</v>
       </c>
@@ -20425,7 +20497,10 @@
         <v>38.557177615571774</v>
       </c>
     </row>
-    <row r="179" spans="2:5">
+    <row r="179" spans="1:5">
+      <c r="A179">
+        <v>178</v>
+      </c>
       <c r="B179">
         <v>276</v>
       </c>
@@ -20439,7 +20514,10 @@
         <v>19.496305953933071</v>
       </c>
     </row>
-    <row r="180" spans="2:5">
+    <row r="180" spans="1:5">
+      <c r="A180">
+        <v>179</v>
+      </c>
       <c r="B180">
         <v>279</v>
       </c>
@@ -20453,7 +20531,10 @@
         <v>17.083406496927129</v>
       </c>
     </row>
-    <row r="181" spans="2:5">
+    <row r="181" spans="1:5">
+      <c r="A181">
+        <v>180</v>
+      </c>
       <c r="B181">
         <v>280</v>
       </c>
@@ -20467,7 +20548,10 @@
         <v>18.280857009781094</v>
       </c>
     </row>
-    <row r="182" spans="2:5">
+    <row r="182" spans="1:5">
+      <c r="A182">
+        <v>181</v>
+      </c>
       <c r="B182">
         <v>281</v>
       </c>
@@ -20481,7 +20565,10 @@
         <v>19.653898152320867</v>
       </c>
     </row>
-    <row r="183" spans="2:5">
+    <row r="183" spans="1:5">
+      <c r="A183">
+        <v>182</v>
+      </c>
       <c r="B183">
         <v>282</v>
       </c>
@@ -20495,7 +20582,10 @@
         <v>17.728406055209259</v>
       </c>
     </row>
-    <row r="184" spans="2:5">
+    <row r="184" spans="1:5">
+      <c r="A184">
+        <v>183</v>
+      </c>
       <c r="B184">
         <v>286</v>
       </c>
@@ -20509,7 +20599,10 @@
         <v>16.847299021692894</v>
       </c>
     </row>
-    <row r="185" spans="2:5">
+    <row r="185" spans="1:5">
+      <c r="A185">
+        <v>184</v>
+      </c>
       <c r="B185">
         <v>287</v>
       </c>
@@ -20523,7 +20616,10 @@
         <v>18.066902968542312</v>
       </c>
     </row>
-    <row r="186" spans="2:5">
+    <row r="186" spans="1:5">
+      <c r="A186">
+        <v>185</v>
+      </c>
       <c r="B186">
         <v>289</v>
       </c>
@@ -20537,7 +20633,10 @@
         <v>18.894869638351555</v>
       </c>
     </row>
-    <row r="187" spans="2:5">
+    <row r="187" spans="1:5">
+      <c r="A187">
+        <v>186</v>
+      </c>
       <c r="B187">
         <v>291</v>
       </c>
@@ -20551,7 +20650,10 @@
         <v>17.265828468792098</v>
       </c>
     </row>
-    <row r="188" spans="2:5">
+    <row r="188" spans="1:5">
+      <c r="A188">
+        <v>187</v>
+      </c>
       <c r="B188">
         <v>292</v>
       </c>
@@ -20565,7 +20667,10 @@
         <v>18.467749210645014</v>
       </c>
     </row>
-    <row r="189" spans="2:5">
+    <row r="189" spans="1:5">
+      <c r="A189">
+        <v>188</v>
+      </c>
       <c r="B189">
         <v>293</v>
       </c>
@@ -20579,7 +20684,10 @@
         <v>16.496183206106871</v>
       </c>
     </row>
-    <row r="190" spans="2:5">
+    <row r="190" spans="1:5">
+      <c r="A190">
+        <v>189</v>
+      </c>
       <c r="B190">
         <v>294</v>
       </c>
@@ -20593,7 +20701,10 @@
         <v>17.638712601994563</v>
       </c>
     </row>
-    <row r="191" spans="2:5">
+    <row r="191" spans="1:5">
+      <c r="A191">
+        <v>190</v>
+      </c>
       <c r="B191">
         <v>295</v>
       </c>
@@ -20607,7 +20718,10 @@
         <v>17.867123287671234</v>
       </c>
     </row>
-    <row r="192" spans="2:5">
+    <row r="192" spans="1:5">
+      <c r="A192">
+        <v>191</v>
+      </c>
       <c r="B192">
         <v>296</v>
       </c>
@@ -20621,7 +20735,10 @@
         <v>18.098742431299488</v>
       </c>
     </row>
-    <row r="193" spans="2:5">
+    <row r="193" spans="1:5">
+      <c r="A193">
+        <v>192</v>
+      </c>
       <c r="B193">
         <v>297</v>
       </c>
@@ -20635,7 +20752,10 @@
         <v>17.39598214285714</v>
       </c>
     </row>
-    <row r="194" spans="2:5">
+    <row r="194" spans="1:5">
+      <c r="A194">
+        <v>193</v>
+      </c>
       <c r="B194">
         <v>298</v>
       </c>
@@ -20649,7 +20769,10 @@
         <v>17.599824484422992</v>
       </c>
     </row>
-    <row r="195" spans="2:5">
+    <row r="195" spans="1:5">
+      <c r="A195">
+        <v>194</v>
+      </c>
       <c r="B195">
         <v>299</v>
       </c>
@@ -20663,7 +20786,10 @@
         <v>17.460026797677536</v>
       </c>
     </row>
-    <row r="196" spans="2:5">
+    <row r="196" spans="1:5">
+      <c r="A196">
+        <v>195</v>
+      </c>
       <c r="B196">
         <v>300</v>
       </c>
@@ -20677,7 +20803,10 @@
         <v>18.070506912442397</v>
       </c>
     </row>
-    <row r="197" spans="2:5">
+    <row r="197" spans="1:5">
+      <c r="A197">
+        <v>196</v>
+      </c>
       <c r="B197">
         <v>301</v>
       </c>
@@ -20691,7 +20820,10 @@
         <v>17.639689071787839</v>
       </c>
     </row>
-    <row r="198" spans="2:5">
+    <row r="198" spans="1:5">
+      <c r="A198">
+        <v>197</v>
+      </c>
       <c r="B198">
         <v>302</v>
       </c>
@@ -20705,7 +20837,10 @@
         <v>16.493915232899706</v>
       </c>
     </row>
-    <row r="199" spans="2:5">
+    <row r="199" spans="1:5">
+      <c r="A199">
+        <v>198</v>
+      </c>
       <c r="B199">
         <v>304</v>
       </c>
@@ -20717,6 +20852,16 @@
       </c>
       <c r="E199" s="1">
         <v>32.064739413680783</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="C200" s="1">
+        <f>AVERAGE(C2:C199)</f>
+        <v>2.5909696969696978</v>
+      </c>
+      <c r="D200" s="1">
+        <f>AVERAGE(D2:D199)</f>
+        <v>49.439722222222223</v>
       </c>
     </row>
   </sheetData>
@@ -20729,8 +20874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB22A503-B58D-B041-B089-126B049701B1}">
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="183" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>